<commit_message>
Aggiorno file need_to_buy.xlsx da R
</commit_message>
<xml_diff>
--- a/need_to_buy.xlsx
+++ b/need_to_buy.xlsx
@@ -1,43 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\EM\SG\ANALISI\ALAIN\dash fcs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4851522-00B8-496A-886D-B820C7639371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t xml:space="preserve">Giorno</t>
+    <t>Giorno</t>
   </si>
   <si>
-    <t xml:space="preserve">TISG_PDR_G</t>
+    <t>TISG_PDR_G</t>
   </si>
   <si>
-    <t xml:space="preserve">fcs</t>
+    <t>fcs</t>
   </si>
   <si>
-    <t xml:space="preserve">buy_BEE_MWH</t>
+    <t>buy_BEE_MWH</t>
   </si>
   <si>
-    <t xml:space="preserve">sell_lago_MWH</t>
+    <t>sell_lago_MWH</t>
   </si>
   <si>
-    <t xml:space="preserve">need_to_buy_MW</t>
+    <t>need_to_buy_MW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -49,6 +69,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,12 +94,21 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -360,14 +390,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,288 +419,288 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>45861</v>
       </c>
-      <c r="B2" t="n">
-        <v>4900.50317639443</v>
-      </c>
-      <c r="C2" t="n">
-        <v>4530.37573689445</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="B2">
+        <v>4900.5031763944298</v>
+      </c>
+      <c r="C2">
+        <v>4530.3757368944498</v>
+      </c>
+      <c r="D2">
         <v>5136</v>
       </c>
-      <c r="E2" t="n">
-        <v>5596.721621</v>
-      </c>
-      <c r="F2" t="n">
-        <v>3.77475756250082</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="E2">
+        <v>5596.7216209999997</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
         <v>45862</v>
       </c>
-      <c r="B3" t="n">
-        <v>4900.50317639443</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4540.55196438533</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="B3">
+        <v>4900.5031763944298</v>
+      </c>
+      <c r="C3">
+        <v>4540.5519643853304</v>
+      </c>
+      <c r="D3">
         <v>2376</v>
       </c>
-      <c r="E3" t="n">
-        <v>5596.721621</v>
-      </c>
-      <c r="F3" t="n">
-        <v>119.198767041288</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="E3">
+        <v>5596.7216209999997</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>45863</v>
       </c>
-      <c r="B4" t="n">
-        <v>4900.50317639443</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4547.35017158116</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="B4">
+        <v>4900.5031763944298</v>
+      </c>
+      <c r="C4">
+        <v>4547.3501715811599</v>
+      </c>
+      <c r="D4">
         <v>2376</v>
       </c>
-      <c r="E4" t="n">
-        <v>5596.721621</v>
-      </c>
-      <c r="F4" t="n">
-        <v>119.482025674447</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="E4">
+        <v>5596.7216209999997</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
         <v>45864</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>1001.82885104655</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>2047.43310592323</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>2376</v>
       </c>
-      <c r="E5" t="n">
-        <v>2104.434169</v>
-      </c>
-      <c r="F5" t="n">
-        <v>32.2516009948615</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="E5">
+        <v>2104.4341690000001</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
         <v>45865</v>
       </c>
-      <c r="B6" t="n">
-        <v>887.939390054798</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="B6">
+        <v>887.93939005479797</v>
+      </c>
+      <c r="C6">
         <v>2003.51940941867</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>2376</v>
       </c>
-      <c r="E6" t="n">
-        <v>1981.503264</v>
-      </c>
-      <c r="F6" t="n">
-        <v>30.0451368068279</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="E6">
+        <v>1981.5032639999999</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>45866</v>
       </c>
-      <c r="B7" t="n">
-        <v>4871.52709026257</v>
-      </c>
-      <c r="C7" t="n">
-        <v>4635.73448628311</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="B7">
+        <v>4871.5270902625698</v>
+      </c>
+      <c r="C7">
+        <v>4635.7344862831096</v>
+      </c>
+      <c r="D7">
         <v>2376</v>
       </c>
-      <c r="E7" t="n">
-        <v>5614.352162</v>
-      </c>
-      <c r="F7" t="n">
-        <v>125.106648250856</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="E7">
+        <v>5614.3521620000001</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
         <v>45867</v>
       </c>
-      <c r="B8" t="n">
-        <v>4871.52709026257</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4606.7988261522</v>
-      </c>
-      <c r="D8" t="n">
+      <c r="B8">
+        <v>4871.5270902625698</v>
+      </c>
+      <c r="C8">
+        <v>4606.7988261521996</v>
+      </c>
+      <c r="D8">
         <v>2376</v>
       </c>
-      <c r="E8" t="n">
-        <v>5614.352162</v>
-      </c>
-      <c r="F8" t="n">
-        <v>123.900995745401</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="E8">
+        <v>5614.3521620000001</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
         <v>45868</v>
       </c>
-      <c r="B9" t="n">
-        <v>4871.52709026257</v>
-      </c>
-      <c r="C9" t="n">
-        <v>4598.80389460356</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="B9">
+        <v>4871.5270902625698</v>
+      </c>
+      <c r="C9">
+        <v>4598.8038946035604</v>
+      </c>
+      <c r="D9">
         <v>2376</v>
       </c>
-      <c r="E9" t="n">
-        <v>5614.352162</v>
-      </c>
-      <c r="F9" t="n">
-        <v>123.567873597541</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="E9">
+        <v>5614.3521620000001</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>45869</v>
       </c>
-      <c r="B10" t="n">
-        <v>4871.52709026257</v>
-      </c>
-      <c r="C10" t="n">
-        <v>4566.35238350058</v>
-      </c>
-      <c r="D10" t="n">
+      <c r="B10">
+        <v>4871.5270902625698</v>
+      </c>
+      <c r="C10">
+        <v>4566.3523835005799</v>
+      </c>
+      <c r="D10">
         <v>2376</v>
       </c>
-      <c r="E10" t="n">
-        <v>5614.352162</v>
-      </c>
-      <c r="F10" t="n">
-        <v>122.215727301584</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="E10">
+        <v>5614.3521620000001</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>45870</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>5314.31945718719</v>
       </c>
-      <c r="C11" t="n">
-        <v>4191.13810354549</v>
-      </c>
-      <c r="D11" t="n">
+      <c r="C11">
+        <v>4191.1381035454897</v>
+      </c>
+      <c r="D11">
         <v>1944</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>5861.381566</v>
       </c>
-      <c r="F11" t="n">
-        <v>116.425008848262</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
         <v>45871</v>
       </c>
-      <c r="B12" t="n">
-        <v>908.164063516383</v>
-      </c>
-      <c r="C12" t="n">
+      <c r="B12">
+        <v>908.16406351638295</v>
+      </c>
+      <c r="C12">
         <v>1517.30073030787</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>1944</v>
       </c>
-      <c r="E12" t="n">
-        <v>1953.728154</v>
-      </c>
-      <c r="F12" t="n">
-        <v>25.7860341996454</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
+      <c r="E12">
+        <v>1953.7281539999999</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
         <v>45872</v>
       </c>
-      <c r="B13" t="n">
-        <v>794.873906828036</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1566.4408225638</v>
-      </c>
-      <c r="D13" t="n">
+      <c r="B13">
+        <v>794.87390682803596</v>
+      </c>
+      <c r="C13">
+        <v>1566.4408225638001</v>
+      </c>
+      <c r="D13">
         <v>1944</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>1829.170294</v>
       </c>
-      <c r="F13" t="n">
-        <v>27.3640504056568</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
+      <c r="F13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
         <v>45873</v>
       </c>
-      <c r="B14" t="n">
-        <v>3947.0732721826</v>
-      </c>
-      <c r="C14" t="n">
-        <v>3921.12784169263</v>
-      </c>
-      <c r="D14" t="n">
+      <c r="B14">
+        <v>3947.0732721825998</v>
+      </c>
+      <c r="C14">
+        <v>3921.1278416926302</v>
+      </c>
+      <c r="D14">
         <v>1944</v>
       </c>
-      <c r="E14" t="n">
-        <v>4608.932317</v>
-      </c>
-      <c r="F14" t="n">
-        <v>109.957786937918</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
+      <c r="E14">
+        <v>4608.9323169999998</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
         <v>45874</v>
       </c>
-      <c r="B15" t="n">
-        <v>3947.0732721826</v>
-      </c>
-      <c r="C15" t="n">
-        <v>3906.72234253067</v>
-      </c>
-      <c r="D15" t="n">
+      <c r="B15">
+        <v>3947.0732721825998</v>
+      </c>
+      <c r="C15">
+        <v>3906.7223425306702</v>
+      </c>
+      <c r="D15">
         <v>1944</v>
       </c>
-      <c r="E15" t="n">
-        <v>4608.932317</v>
-      </c>
-      <c r="F15" t="n">
-        <v>109.35755780617</v>
+      <c r="E15">
+        <v>4608.9323169999998</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>